<commit_message>
upload corrected version of results of Exercises 4
</commit_message>
<xml_diff>
--- a/files/QT/Exercises_4_results.xlsx
+++ b/files/QT/Exercises_4_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500" firstSheet="5" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise 1" sheetId="6" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -748,26 +748,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,6 +766,15 @@
     </xf>
     <xf numFmtId="10" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -921,6 +921,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1002,13 +1007,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31070801638385</c:v>
+                  <c:v>0.310344827586207</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.629022820362785</c:v>
+                  <c:v>0.628647214854111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.899356348741954</c:v>
+                  <c:v>0.89920424403183</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.0</c:v>
@@ -1089,11 +1094,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130221784"/>
-        <c:axId val="2129185192"/>
+        <c:axId val="2108573464"/>
+        <c:axId val="2108574888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130221784"/>
+        <c:axId val="2108573464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1104,12 +1109,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129185192"/>
+        <c:crossAx val="2108574888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2129185192"/>
+        <c:axId val="2108574888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1120,7 +1125,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130221784"/>
+        <c:crossAx val="2108573464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1152,7 +1157,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1240,11 +1244,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2132178328"/>
-        <c:axId val="2127135592"/>
+        <c:axId val="2065515032"/>
+        <c:axId val="2065518072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2132178328"/>
+        <c:axId val="2065515032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1267,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127135592"/>
+        <c:crossAx val="2065518072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1271,7 +1275,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127135592"/>
+        <c:axId val="2065518072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,7 +1286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132178328"/>
+        <c:crossAx val="2065515032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1314,7 +1318,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1402,11 +1405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2128858776"/>
-        <c:axId val="2131939304"/>
+        <c:axId val="2108636392"/>
+        <c:axId val="2108639432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2128858776"/>
+        <c:axId val="2108636392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131939304"/>
+        <c:crossAx val="2108639432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1433,7 +1436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131939304"/>
+        <c:axId val="2108639432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,7 +1447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128858776"/>
+        <c:crossAx val="2108636392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1961,11 +1964,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2126044120"/>
-        <c:axId val="2126047064"/>
+        <c:axId val="2107953576"/>
+        <c:axId val="2107950680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2126044120"/>
+        <c:axId val="2107953576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,12 +1978,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126047064"/>
+        <c:crossAx val="2107950680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2126047064"/>
+        <c:axId val="2107950680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,7 +1994,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126044120"/>
+        <c:crossAx val="2107953576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2473,13 +2476,13 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
@@ -2616,7 +2619,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2629,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3118,10 +3120,10 @@
       <c r="H39" t="s">
         <v>70</v>
       </c>
-      <c r="I39" s="26" t="s">
+      <c r="I39" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="J39" s="26" t="s">
+      <c r="J39" s="24" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3132,11 +3134,11 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" s="28">
+      <c r="I40" s="26">
         <f>G40/G$44</f>
         <v>0</v>
       </c>
-      <c r="J40" s="28">
+      <c r="J40" s="26">
         <f>H40/H$44</f>
         <v>0</v>
       </c>
@@ -3157,8 +3159,8 @@
         <v>9</v>
       </c>
       <c r="F41">
-        <f>(A41+50)*D41</f>
-        <v>5310</v>
+        <f>(A41+45)*D41</f>
+        <v>5265</v>
       </c>
       <c r="G41">
         <f>D41</f>
@@ -3166,15 +3168,15 @@
       </c>
       <c r="H41">
         <f>F41</f>
-        <v>5310</v>
-      </c>
-      <c r="I41" s="28">
+        <v>5265</v>
+      </c>
+      <c r="I41" s="26">
         <f t="shared" ref="I41:J44" si="5">G41/G$44</f>
         <v>0.36</v>
       </c>
-      <c r="J41" s="28">
+      <c r="J41" s="26">
         <f t="shared" si="5"/>
-        <v>0.31070801638385021</v>
+        <v>0.31034482758620691</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -3193,8 +3195,8 @@
         <v>8</v>
       </c>
       <c r="F42">
-        <f t="shared" ref="F42:F44" si="6">(A42+50)*D42</f>
-        <v>5440</v>
+        <f>(A42+45)*D42</f>
+        <v>5400</v>
       </c>
       <c r="G42">
         <f>D42+G41</f>
@@ -3202,15 +3204,15 @@
       </c>
       <c r="H42">
         <f>F42+H41</f>
-        <v>10750</v>
-      </c>
-      <c r="I42" s="28">
+        <v>10665</v>
+      </c>
+      <c r="I42" s="26">
         <f t="shared" si="5"/>
         <v>0.68</v>
       </c>
-      <c r="J42" s="28">
+      <c r="J42" s="26">
         <f t="shared" si="5"/>
-        <v>0.62902282036278523</v>
+        <v>0.62864721485411146</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3229,24 +3231,24 @@
         <v>6</v>
       </c>
       <c r="F43">
-        <f t="shared" si="6"/>
-        <v>4620</v>
+        <f>(A43+45)*D43</f>
+        <v>4590</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43:G44" si="7">D43+G42</f>
+        <f t="shared" ref="G43:G44" si="6">D43+G42</f>
         <v>23</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:H44" si="8">F43+H42</f>
-        <v>15370</v>
-      </c>
-      <c r="I43" s="28">
+        <f t="shared" ref="H43:H44" si="7">F43+H42</f>
+        <v>15255</v>
+      </c>
+      <c r="I43" s="26">
         <f t="shared" si="5"/>
         <v>0.92</v>
       </c>
-      <c r="J43" s="28">
+      <c r="J43" s="26">
         <f t="shared" si="5"/>
-        <v>0.89935634874195436</v>
+        <v>0.89920424403183019</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3265,22 +3267,22 @@
         <v>2</v>
       </c>
       <c r="F44">
+        <f>(A44+45)*D44</f>
+        <v>1710</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="6"/>
-        <v>1720</v>
-      </c>
-      <c r="G44">
+        <v>25</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="8"/>
-        <v>17090</v>
-      </c>
-      <c r="I44" s="28">
+        <v>16965</v>
+      </c>
+      <c r="I44" s="26">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="J44" s="28">
+      <c r="J44" s="26">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -3302,7 +3304,7 @@
       </c>
       <c r="B47">
         <f>SUM(F41:F44)/SUM(D41:D44)</f>
-        <v>683.6</v>
+        <v>678.6</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -3352,8 +3354,8 @@
         <v>67</v>
       </c>
       <c r="D55">
-        <f>A43+90*7/8</f>
-        <v>798.75</v>
+        <f>A43+90*5/6</f>
+        <v>795</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3371,7 +3373,7 @@
       </c>
       <c r="D57">
         <f>(D55+D56)/2</f>
-        <v>804.375</v>
+        <v>802.5</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3383,7 +3385,7 @@
       <c r="A60" t="s">
         <v>74</v>
       </c>
-      <c r="D60" s="29">
+      <c r="D60" s="27">
         <f>D29/D24</f>
         <v>2.7105263157894739</v>
       </c>
@@ -3392,47 +3394,47 @@
       <c r="A61" t="s">
         <v>73</v>
       </c>
-      <c r="D61" s="29">
+      <c r="D61" s="27">
         <f>D57/D54</f>
-        <v>1.4236725663716814</v>
+        <v>1.4203539823008851</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
     </row>
     <row r="64" spans="1:7">
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
     </row>
     <row r="66" spans="1:7">
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="22" t="s">
@@ -3448,54 +3450,54 @@
       <c r="A70" t="s">
         <v>79</v>
       </c>
-      <c r="B70" s="29">
+      <c r="B70" s="27">
         <f>I41*J41/2</f>
-        <v>5.5927442949093034E-2</v>
+        <v>5.5862068965517243E-2</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>80</v>
       </c>
-      <c r="B71" s="29">
+      <c r="B71" s="27">
         <f>(J41+J42)*(I42-I41)/2</f>
-        <v>0.1503569338794617</v>
+        <v>0.15023872679045097</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>81</v>
       </c>
-      <c r="B72" s="29">
+      <c r="B72" s="27">
         <f>(J43+J42)*(I43-I42)/2</f>
-        <v>0.18340550029256875</v>
+        <v>0.18334217506631301</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>82</v>
       </c>
-      <c r="B73" s="29">
+      <c r="B73" s="27">
         <f>(J44+J43)*(I44-I43)/2</f>
-        <v>7.5974253949678147E-2</v>
+        <v>7.5968169761273172E-2</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>83</v>
       </c>
-      <c r="B74" s="29">
+      <c r="B74" s="27">
         <f>SUM(B70:B73)</f>
-        <v>0.46566413107080162</v>
+        <v>0.46541114058355437</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="29">
+      <c r="B76" s="27">
         <f>1-2*B74</f>
-        <v>6.8671737858396753E-2</v>
+        <v>6.9177718832891255E-2</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3511,7 +3513,6 @@
     <mergeCell ref="B63:G66"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3548,7 +3549,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>0.06</v>
       </c>
       <c r="C4">
@@ -3556,7 +3557,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C5">
@@ -3564,7 +3565,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="B6" s="28">
+      <c r="B6" s="26">
         <v>0.08</v>
       </c>
       <c r="C6">
@@ -3575,47 +3576,47 @@
       <c r="B7" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="25">
         <f>(1+B4)^(C4/10)*(1+B5)^(C5/10)*(1+B6)^(C6/10)-1</f>
         <v>6.8967757404103658E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
@@ -3652,7 +3653,7 @@
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="31">
         <f t="shared" si="0"/>
         <v>11910.16</v>
       </c>
@@ -3661,7 +3662,7 @@
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="31">
         <f t="shared" si="0"/>
         <v>12624.7696</v>
       </c>
@@ -3670,7 +3671,7 @@
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="31">
         <f>B18*(1+$B$5)</f>
         <v>13508.503472</v>
       </c>
@@ -3679,7 +3680,7 @@
       <c r="A20">
         <v>6</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="31">
         <f t="shared" ref="B20:B21" si="1">B19*(1+$B$5)</f>
         <v>14454.098715040001</v>
       </c>
@@ -3688,7 +3689,7 @@
       <c r="A21">
         <v>7</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="31">
         <f t="shared" si="1"/>
         <v>15465.885625092802</v>
       </c>
@@ -3697,7 +3698,7 @@
       <c r="A22">
         <v>8</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="31">
         <f>B21*(1+$B$6)</f>
         <v>16703.156475100226</v>
       </c>
@@ -3706,7 +3707,7 @@
       <c r="A23">
         <v>9</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="31">
         <f t="shared" ref="B23:B24" si="2">B22*(1+$B$6)</f>
         <v>18039.408993108245</v>
       </c>
@@ -3715,7 +3716,7 @@
       <c r="A24">
         <v>10</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="32">
         <f t="shared" si="2"/>
         <v>19482.561712556908</v>
       </c>
@@ -3729,10 +3730,10 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="34">
         <f>(B24/B14)^(1/10)-1</f>
         <v>6.8967757404103658E-2</v>
       </c>
@@ -3888,11 +3889,11 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="30">
         <f>AVERAGE(C2:C6)</f>
         <v>13</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="30">
         <f>AVERAGE(E2:E6)</f>
         <v>13</v>
       </c>
@@ -3953,7 +3954,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3984,15 +3984,15 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="E1" s="38"/>
+      <c r="G1" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" t="s">
         <v>100</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>3</v>
       </c>
       <c r="G3">
-        <f>($A3+$A4)/2*D3</f>
+        <f t="shared" ref="G3:G8" si="0">($A3+$A4)/2*D3</f>
         <v>150000</v>
       </c>
       <c r="H3" t="e">
@@ -4085,11 +4085,11 @@
         <f>E3</f>
         <v>30</v>
       </c>
-      <c r="L3" s="38">
+      <c r="L3" s="35">
         <f>G3</f>
         <v>150000</v>
       </c>
-      <c r="M3" s="38">
+      <c r="M3" s="35">
         <f>I3</f>
         <v>750000</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>30000</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B8" si="0">CONCATENATE(A4," - ",A5)</f>
+        <f t="shared" ref="B4:B8" si="1">CONCATENATE(A4," - ",A5)</f>
         <v>30000 - 40000</v>
       </c>
       <c r="C4" t="s">
@@ -4123,7 +4123,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <f>($A4+$A5)/2*D4</f>
+        <f t="shared" si="0"/>
         <v>560000</v>
       </c>
       <c r="H4" t="e">
@@ -4131,7 +4131,7 @@
         <v>#REF!</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I8" si="1">($A4+$A5)/2*E4</f>
+        <f t="shared" ref="I4:I8" si="2">($A4+$A5)/2*E4</f>
         <v>735000</v>
       </c>
       <c r="J4">
@@ -4142,11 +4142,11 @@
         <f>E4+K3</f>
         <v>51</v>
       </c>
-      <c r="L4" s="38">
+      <c r="L4" s="35">
         <f>G4+L3</f>
         <v>710000</v>
       </c>
-      <c r="M4" s="38">
+      <c r="M4" s="35">
         <f>I4+M3</f>
         <v>1485000</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>278890000</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O8" si="2">(($A4+$A5)/2-E$10)^2</f>
+        <f t="shared" ref="O4:O8" si="3">(($A4+$A5)/2-E$10)^2</f>
         <v>46240000</v>
       </c>
     </row>
@@ -4164,7 +4164,7 @@
         <v>40000</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40000 - 50000</v>
       </c>
       <c r="C5" t="s">
@@ -4180,7 +4180,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <f>($A5+$A6)/2*D5</f>
+        <f t="shared" si="0"/>
         <v>1125000</v>
       </c>
       <c r="H5" t="e">
@@ -4188,7 +4188,7 @@
         <v>#REF!</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>990000</v>
       </c>
       <c r="J5">
@@ -4196,14 +4196,14 @@
         <v>47</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K8" si="3">E5+K4</f>
+        <f t="shared" ref="K5:K8" si="4">E5+K4</f>
         <v>73</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="35">
         <f>G5+L4</f>
         <v>1835000</v>
       </c>
-      <c r="M5" s="38">
+      <c r="M5" s="35">
         <f>I5+M4</f>
         <v>2475000</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>44890000</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10240000</v>
       </c>
     </row>
@@ -4221,7 +4221,7 @@
         <v>50000</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50000 - 60000</v>
       </c>
       <c r="C6" t="s">
@@ -4237,7 +4237,7 @@
         <v>3</v>
       </c>
       <c r="G6">
-        <f>($A6+$A7)/2*D6</f>
+        <f t="shared" si="0"/>
         <v>1210000</v>
       </c>
       <c r="H6" t="e">
@@ -4245,7 +4245,7 @@
         <v>#REF!</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>715000</v>
       </c>
       <c r="J6">
@@ -4253,14 +4253,14 @@
         <v>69</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
-      <c r="L6" s="38">
+      <c r="L6" s="35">
         <f>G6+L5</f>
         <v>3045000</v>
       </c>
-      <c r="M6" s="38">
+      <c r="M6" s="35">
         <f>I6+M5</f>
         <v>3190000</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>10890000</v>
       </c>
       <c r="O6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>174240000</v>
       </c>
     </row>
@@ -4278,7 +4278,7 @@
         <v>60000</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60000 - 70000</v>
       </c>
       <c r="C7" t="s">
@@ -4294,7 +4294,7 @@
         <v>3</v>
       </c>
       <c r="G7">
-        <f>($A7+$A8)/2*D7</f>
+        <f t="shared" si="0"/>
         <v>1300000</v>
       </c>
       <c r="H7" t="e">
@@ -4302,7 +4302,7 @@
         <v>#REF!</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>390000</v>
       </c>
       <c r="J7">
@@ -4310,14 +4310,14 @@
         <v>89</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="L7" s="38">
+      <c r="L7" s="35">
         <f>G7+L6</f>
         <v>4345000</v>
       </c>
-      <c r="M7" s="38">
+      <c r="M7" s="35">
         <f>I7+M6</f>
         <v>3580000</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>176890000</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>538240000</v>
       </c>
     </row>
@@ -4335,7 +4335,7 @@
         <v>70000</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70000 - 80000</v>
       </c>
       <c r="C8" t="s">
@@ -4351,7 +4351,7 @@
         <v>3</v>
       </c>
       <c r="G8">
-        <f>($A8+$A9)/2*D8</f>
+        <f t="shared" si="0"/>
         <v>825000</v>
       </c>
       <c r="H8" t="e">
@@ -4359,7 +4359,7 @@
         <v>#REF!</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>600000</v>
       </c>
       <c r="J8">
@@ -4367,14 +4367,14 @@
         <v>100</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="35">
         <f>G8+L7</f>
         <v>5170000</v>
       </c>
-      <c r="M8" s="38">
+      <c r="M8" s="35">
         <f>I8+M7</f>
         <v>4180000</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>542890000</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1102240000</v>
       </c>
     </row>
@@ -4396,11 +4396,11 @@
       <c r="B10" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="35">
         <f>SUM(G3:G8)/SUM(D3:D8)</f>
         <v>51700</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="35">
         <f>SUM(I3:I8)/SUM(E3:E8)</f>
         <v>41800</v>
       </c>
@@ -4409,11 +4409,11 @@
       <c r="B11" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="35">
         <f>A6+10000*3/D6</f>
         <v>51363.63636363636</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="35">
         <f>A4+10000*1/E4</f>
         <v>30476.190476190477</v>
       </c>
@@ -4447,7 +4447,6 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4962,7 +4961,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5205,7 +5203,7 @@
       <c r="D16" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="28">
         <f>CORREL(A2:A71,B2:B71)</f>
         <v>0.65915012743002421</v>
       </c>
@@ -5254,7 +5252,7 @@
       <c r="D20" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <f>F16^2</f>
         <v>0.43447889049101718</v>
       </c>
@@ -5741,7 +5739,6 @@
     <sortCondition ref="D3"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
update of Lecture 5 - minor changes on harmonic mean
</commit_message>
<xml_diff>
--- a/files/QT/Exercises_4_results.xlsx
+++ b/files/QT/Exercises_4_results.xlsx
@@ -707,7 +707,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -775,6 +775,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2631,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2948,7 +2950,7 @@
         <v>1900</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
+        <f>H10+I9</f>
         <v>29500</v>
       </c>
     </row>
@@ -3009,7 +3011,7 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="39">
         <f>A4+1/9*(A5-A4)</f>
         <v>311.11111111111109</v>
       </c>
@@ -3018,7 +3020,7 @@
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="39">
         <f>A4+2/9*(A5-A4)</f>
         <v>322.22222222222223</v>
       </c>
@@ -3029,7 +3031,7 @@
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="20">
+      <c r="D24" s="40">
         <f>(D23+D22)/2</f>
         <v>316.66666666666663</v>
       </c>

</xml_diff>

<commit_message>
Correction of Exercises 4
</commit_message>
<xml_diff>
--- a/files/QT/Exercises_4_results.xlsx
+++ b/files/QT/Exercises_4_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise 1" sheetId="6" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Exercise 6" sheetId="4" r:id="rId6"/>
     <sheet name="Exercise 7" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -434,6 +434,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -462,28 +463,33 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="3" tint="0.39997558519241921"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="6" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -491,6 +497,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -766,6 +773,8 @@
     </xf>
     <xf numFmtId="10" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -775,150 +784,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="141">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -934,7 +941,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -982,7 +989,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.36</c:v>
@@ -994,7 +1001,7 @@
                   <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1006,19 +1013,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.310344827586207</c:v>
+                  <c:v>0.31034482758620691</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.628647214854111</c:v>
+                  <c:v>0.62864721485411146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89920424403183</c:v>
+                  <c:v>0.89920424403183019</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1045,7 +1052,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.36</c:v>
@@ -1057,7 +1064,7 @@
                   <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1069,7 +1076,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.36</c:v>
@@ -1081,7 +1088,7 @@
                   <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,14 +1103,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2108573464"/>
-        <c:axId val="2108574888"/>
+        <c:axId val="79387648"/>
+        <c:axId val="75571968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2108573464"/>
+        <c:axId val="79387648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1111,15 +1118,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108574888"/>
+        <c:crossAx val="75571968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2108574888"/>
+        <c:axId val="75571968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1127,7 +1134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108573464"/>
+        <c:crossAx val="79387648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1138,7 +1145,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1147,7 +1154,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1216,22 +1223,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,11 +1253,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2065515032"/>
-        <c:axId val="2065518072"/>
+        <c:axId val="79970688"/>
+        <c:axId val="79972224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2065515032"/>
+        <c:axId val="79970688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1266,10 +1273,10 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2065518072"/>
+        <c:crossAx val="79972224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1277,7 +1284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2065518072"/>
+        <c:axId val="79972224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1288,7 +1295,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065515032"/>
+        <c:crossAx val="79970688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1299,7 +1306,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1308,7 +1315,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1377,22 +1384,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1407,11 +1414,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2108636392"/>
-        <c:axId val="2108639432"/>
+        <c:axId val="79996416"/>
+        <c:axId val="79997952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2108636392"/>
+        <c:axId val="79996416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,10 +1434,10 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108639432"/>
+        <c:crossAx val="79997952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1438,7 +1445,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108639432"/>
+        <c:axId val="79997952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1456,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108636392"/>
+        <c:crossAx val="79996416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1460,7 +1467,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1469,7 +1476,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1501,8 +1508,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.287224222683739"/>
-                  <c:y val="-0.298097747452748"/>
+                  <c:x val="-0.28722422268373898"/>
+                  <c:y val="-0.29809774745274797"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1513,7 +1520,7 @@
                   <a:pPr>
                     <a:defRPr b="1"/>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="fr-FR"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1525,214 +1532,214 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="0">
-                  <c:v>357.0</c:v>
+                  <c:v>357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>932.0</c:v>
+                  <c:v>932</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>366.0</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.0</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>67.0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>413.0</c:v>
+                  <c:v>413</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>496.0</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>458.0</c:v>
+                  <c:v>458</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>152.0</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>115.0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>964.0</c:v>
+                  <c:v>964</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>459.0</c:v>
+                  <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>421.0</c:v>
+                  <c:v>421</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>723.0</c:v>
+                  <c:v>723</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>294.0</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1310.0</c:v>
+                  <c:v>1310</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>627.0</c:v>
+                  <c:v>627</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>714.0</c:v>
+                  <c:v>714</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>270.0</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>71.0</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>135.0</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>182.0</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>82.0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1137.0</c:v>
+                  <c:v>1137</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>195.0</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>325.0</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>282.0</c:v>
+                  <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>228.0</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>351.0</c:v>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1541.0</c:v>
+                  <c:v>1541</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1661.0</c:v>
+                  <c:v>1661</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2769.0</c:v>
+                  <c:v>2769</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>510.0</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>678.0</c:v>
+                  <c:v>678</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1113.0</c:v>
+                  <c:v>1113</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2178.0</c:v>
+                  <c:v>2178</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1074.0</c:v>
+                  <c:v>1074</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>586.0</c:v>
+                  <c:v>586</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2232.0</c:v>
+                  <c:v>2232</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>92.0</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>640.0</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2663.0</c:v>
+                  <c:v>2663</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>925.0</c:v>
+                  <c:v>925</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>503.0</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>472.0</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>346.0</c:v>
+                  <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>337.0</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>993.0</c:v>
+                  <c:v>993</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1575.0</c:v>
+                  <c:v>1575</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2501.0</c:v>
+                  <c:v>2501</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2304.0</c:v>
+                  <c:v>2304</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2493.0</c:v>
+                  <c:v>2493</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>71.0</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>185.0</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>327.0</c:v>
+                  <c:v>327</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>409.0</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>117.0</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>179.0</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>234.0</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1759,10 +1766,10 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.6</c:v>
@@ -1777,7 +1784,7 @@
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.9</c:v>
@@ -1786,13 +1793,13 @@
                   <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.5</c:v>
@@ -1840,7 +1847,7 @@
                   <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.6</c:v>
@@ -1852,7 +1859,7 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>2.9</c:v>
@@ -1861,7 +1868,7 @@
                   <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0.9</c:v>
@@ -1876,7 +1883,7 @@
                   <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>1.8</c:v>
@@ -1891,13 +1898,13 @@
                   <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>1.2</c:v>
@@ -1933,7 +1940,7 @@
                   <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.1</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>0.6</c:v>
@@ -1966,11 +1973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2107953576"/>
-        <c:axId val="2107950680"/>
+        <c:axId val="80201216"/>
+        <c:axId val="80202752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2107953576"/>
+        <c:axId val="80201216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,12 +1987,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107950680"/>
+        <c:crossAx val="80202752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2107950680"/>
+        <c:axId val="80202752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +2003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107953576"/>
+        <c:crossAx val="80201216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2007,7 +2014,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2478,18 +2485,18 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="17.625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
@@ -2497,7 +2504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -2505,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -2513,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="12">
         <v>3</v>
       </c>
@@ -2521,7 +2528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
         <v>5</v>
       </c>
@@ -2529,7 +2536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
         <v>8</v>
       </c>
@@ -2537,7 +2544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
         <v>10</v>
       </c>
@@ -2545,7 +2552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
         <v>12</v>
       </c>
@@ -2553,7 +2560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
         <v>13</v>
       </c>
@@ -2561,13 +2568,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="13">
         <v>15</v>
       </c>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -2580,7 +2587,7 @@
         <v>9.875</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
@@ -2593,7 +2600,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>29</v>
       </c>
@@ -2606,7 +2613,7 @@
         <v>5.59375</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
@@ -2634,22 +2641,22 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.83203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="9" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1">
+    <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
@@ -2672,7 +2679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -2702,7 +2709,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -2732,7 +2739,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
@@ -2761,11 +2768,11 @@
         <v>1750</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I10" si="3">H4+I3</f>
+        <f t="shared" ref="I4:I9" si="3">H4+I3</f>
         <v>2550</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>400</v>
       </c>
@@ -2795,7 +2802,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
@@ -2828,7 +2835,7 @@
         <v>10650</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>600</v>
       </c>
@@ -2861,7 +2868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>700</v>
       </c>
@@ -2891,7 +2898,7 @@
         <v>22500</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>800</v>
       </c>
@@ -2924,7 +2931,7 @@
         <v>27600</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>900</v>
       </c>
@@ -2954,7 +2961,7 @@
         <v>29500</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>1000</v>
       </c>
@@ -2963,22 +2970,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2987,61 +2994,61 @@
         <v>590</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="39">
-        <f>A4+1/9*(A5-A4)</f>
-        <v>311.11111111111109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="36">
+        <f>A4+1/D4*(A5-A4)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="39">
-        <f>A4+2/9*(A5-A4)</f>
-        <v>322.22222222222223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" s="36">
+        <f>A4+2/D4*(A5-A4)</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="40">
+      <c r="D24" s="37">
         <f>(D23+D22)/2</f>
-        <v>316.66666666666663</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -3050,7 +3057,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -3059,7 +3066,7 @@
         <v>866.66666666666663</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>50</v>
       </c>
@@ -3070,17 +3077,17 @@
         <v>858.33333333333326</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -3089,7 +3096,7 @@
         <v>29500</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3098,7 +3105,7 @@
         <v>14750</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -3107,12 +3114,12 @@
         <v>670.08547008547009</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -3129,7 +3136,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G40">
         <v>0</v>
       </c>
@@ -3145,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>A7*0.9</f>
         <v>540</v>
@@ -3181,7 +3188,7 @@
         <v>0.31034482758620691</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>A8*0.9</f>
         <v>630</v>
@@ -3217,7 +3224,7 @@
         <v>0.62864721485411146</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>A9*0.9</f>
         <v>720</v>
@@ -3253,7 +3260,7 @@
         <v>0.89920424403183019</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>A10*0.9</f>
         <v>810</v>
@@ -3289,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="23">
         <f>A11*0.9</f>
         <v>900</v>
@@ -3300,7 +3307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -3309,22 +3316,22 @@
         <v>678.6</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -3333,7 +3340,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -3342,7 +3349,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -3351,7 +3358,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -3360,7 +3367,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -3369,7 +3376,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -3378,21 +3385,21 @@
         <v>802.5</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="27">
         <f>D29/D24</f>
-        <v>2.7105263157894739</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>2.6010101010101008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3401,54 +3408,54 @@
         <v>1.4203539823008851</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="36" t="s">
+      <c r="B63" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -3457,7 +3464,7 @@
         <v>5.5862068965517243E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -3466,7 +3473,7 @@
         <v>0.15023872679045097</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -3475,7 +3482,7 @@
         <v>0.18334217506631301</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -3484,7 +3491,7 @@
         <v>7.5968169761273172E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -3493,7 +3500,7 @@
         <v>0.46541114058355437</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -3502,7 +3509,7 @@
         <v>6.9177718832891255E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>85</v>
       </c>
@@ -3532,17 +3539,17 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>89</v>
       </c>
@@ -3550,7 +3557,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="26">
         <v>0.06</v>
       </c>
@@ -3558,7 +3565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="26">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -3566,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="26">
         <v>0.08</v>
       </c>
@@ -3574,7 +3581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>95</v>
       </c>
@@ -3583,36 +3590,36 @@
         <v>6.8967757404103658E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -3620,12 +3627,12 @@
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -3633,7 +3640,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -3642,7 +3649,7 @@
         <v>10600</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3651,7 +3658,7 @@
         <v>11236</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3660,7 +3667,7 @@
         <v>11910.16</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -3669,7 +3676,7 @@
         <v>12624.7696</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -3678,7 +3685,7 @@
         <v>13508.503472</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -3687,7 +3694,7 @@
         <v>14454.098715040001</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -3696,7 +3703,7 @@
         <v>15465.885625092802</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -3705,7 +3712,7 @@
         <v>16703.156475100226</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -3714,7 +3721,7 @@
         <v>18039.408993108245</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -3723,7 +3730,7 @@
         <v>19482.561712556908</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -3731,7 +3738,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>94</v>
       </c>
@@ -3761,16 +3768,16 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="2.625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -3787,7 +3794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3807,7 +3814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3827,7 +3834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3847,7 +3854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3867,7 +3874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3887,7 +3894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3900,7 +3907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3913,7 +3920,7 @@
         <v>2.2803508501982761</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3934,22 +3941,22 @@
         <v>0.17541160386140586</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -3972,29 +3979,29 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="2.625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="G1" s="38" t="s">
+      <c r="E1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="J1" t="s">
         <v>100</v>
       </c>
@@ -4005,7 +4012,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>15</v>
       </c>
@@ -4047,7 +4054,7 @@
         <v>Sales</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20000</v>
       </c>
@@ -4104,7 +4111,7 @@
         <v>282240000</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30000</v>
       </c>
@@ -4161,7 +4168,7 @@
         <v>46240000</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40000</v>
       </c>
@@ -4218,7 +4225,7 @@
         <v>10240000</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50000</v>
       </c>
@@ -4275,7 +4282,7 @@
         <v>174240000</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60000</v>
       </c>
@@ -4332,7 +4339,7 @@
         <v>538240000</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70000</v>
       </c>
@@ -4389,12 +4396,12 @@
         <v>1102240000</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80000</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>99</v>
       </c>
@@ -4407,7 +4414,7 @@
         <v>41800</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -4420,7 +4427,7 @@
         <v>30476.190476190477</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -4433,12 +4440,12 @@
         <v>15484.185480676728</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>104</v>
       </c>
@@ -4466,19 +4473,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="2.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="2.625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="2.875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="2.875" customWidth="1"/>
+    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -4504,7 +4511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4540,7 +4547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -4576,7 +4583,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -4612,7 +4619,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -4648,7 +4655,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40</v>
       </c>
@@ -4684,7 +4691,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -4720,7 +4727,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60</v>
       </c>
@@ -4756,7 +4763,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70</v>
       </c>
@@ -4792,7 +4799,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>80</v>
       </c>
@@ -4828,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90</v>
       </c>
@@ -4864,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -4880,12 +4887,12 @@
         <v>39.696969696969695</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f>J1</f>
         <v>Speedy</v>
@@ -4895,7 +4902,7 @@
         <v>Peach</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>105</v>
       </c>
@@ -4909,7 +4916,7 @@
         <v>39.696969696969695</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>106</v>
       </c>
@@ -4923,7 +4930,7 @@
         <v>20 - 30</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>108</v>
       </c>
@@ -4937,7 +4944,7 @@
         <v>40 - 50</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>107</v>
       </c>
@@ -4951,12 +4958,12 @@
         <v>50 - 60</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>109</v>
       </c>
@@ -4979,16 +4986,16 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
@@ -4997,7 +5004,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0.7</v>
       </c>
@@ -5012,7 +5019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>0.7</v>
       </c>
@@ -5032,7 +5039,7 @@
         <v>639.42700000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.8</v>
       </c>
@@ -5052,7 +5059,7 @@
         <v>721.13317186088648</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.7</v>
       </c>
@@ -5072,7 +5079,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.8</v>
       </c>
@@ -5092,7 +5099,7 @@
         <v>2769</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -5101,7 +5108,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>0</v>
       </c>
@@ -5113,7 +5120,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.6</v>
       </c>
@@ -5125,7 +5132,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>0.3</v>
       </c>
@@ -5137,7 +5144,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
@@ -5149,7 +5156,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>0.4</v>
       </c>
@@ -5161,7 +5168,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
@@ -5173,7 +5180,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>0.9</v>
       </c>
@@ -5182,7 +5189,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>1.2</v>
       </c>
@@ -5194,7 +5201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
@@ -5210,7 +5217,7 @@
         <v>0.65915012743002421</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1.3</v>
       </c>
@@ -5222,7 +5229,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -5231,7 +5238,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.5</v>
       </c>
@@ -5243,7 +5250,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.7</v>
       </c>
@@ -5259,7 +5266,7 @@
         <v>0.43447889049101718</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0.6</v>
       </c>
@@ -5271,7 +5278,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1.4</v>
       </c>
@@ -5283,7 +5290,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.6</v>
       </c>
@@ -5301,7 +5308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.4</v>
       </c>
@@ -5313,7 +5320,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0.2</v>
       </c>
@@ -5322,7 +5329,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>0.4</v>
       </c>
@@ -5331,7 +5338,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>0.6</v>
       </c>
@@ -5340,7 +5347,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>0.6</v>
       </c>
@@ -5349,7 +5356,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.7</v>
       </c>
@@ -5358,7 +5365,7 @@
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>0.5</v>
       </c>
@@ -5367,7 +5374,7 @@
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>1.3</v>
       </c>
@@ -5376,7 +5383,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>0.7</v>
       </c>
@@ -5385,7 +5392,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>1.2</v>
       </c>
@@ -5394,7 +5401,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>1</v>
       </c>
@@ -5403,7 +5410,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>0.6</v>
       </c>
@@ -5412,7 +5419,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>0.8</v>
       </c>
@@ -5421,7 +5428,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>0.6</v>
       </c>
@@ -5430,7 +5437,7 @@
       </c>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>1</v>
       </c>
@@ -5439,7 +5446,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>2.9</v>
       </c>
@@ -5448,7 +5455,7 @@
       </c>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>1.3</v>
       </c>
@@ -5457,7 +5464,7 @@
       </c>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>1</v>
       </c>
@@ -5466,7 +5473,7 @@
       </c>
       <c r="C41" s="5"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>0.9</v>
       </c>
@@ -5475,7 +5482,7 @@
       </c>
       <c r="C42" s="5"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>1.2</v>
       </c>
@@ -5484,7 +5491,7 @@
       </c>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>2.9</v>
       </c>
@@ -5493,7 +5500,7 @@
       </c>
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>1.4</v>
       </c>
@@ -5502,7 +5509,7 @@
       </c>
       <c r="C45" s="5"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>1</v>
       </c>
@@ -5511,7 +5518,7 @@
       </c>
       <c r="C46" s="5"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>1.8</v>
       </c>
@@ -5520,7 +5527,7 @@
       </c>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>2.9</v>
       </c>
@@ -5529,7 +5536,7 @@
       </c>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>0.3</v>
       </c>
@@ -5538,7 +5545,7 @@
       </c>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>2.6</v>
       </c>
@@ -5547,7 +5554,7 @@
       </c>
       <c r="C50" s="5"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>2</v>
       </c>
@@ -5556,7 +5563,7 @@
       </c>
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>1.6</v>
       </c>
@@ -5565,7 +5572,7 @@
       </c>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>2</v>
       </c>
@@ -5574,7 +5581,7 @@
       </c>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>1.2</v>
       </c>
@@ -5583,7 +5590,7 @@
       </c>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>1.7</v>
       </c>
@@ -5592,7 +5599,7 @@
       </c>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>1.7</v>
       </c>
@@ -5601,7 +5608,7 @@
       </c>
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>0.2</v>
       </c>
@@ -5610,7 +5617,7 @@
       </c>
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>0.9</v>
       </c>
@@ -5619,7 +5626,7 @@
       </c>
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>2.5</v>
       </c>
@@ -5628,7 +5635,7 @@
       </c>
       <c r="C59" s="5"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>0.1</v>
       </c>
@@ -5637,7 +5644,7 @@
       </c>
       <c r="C60" s="5"/>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>3.9</v>
       </c>
@@ -5646,7 +5653,7 @@
       </c>
       <c r="C61" s="5"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>5.3</v>
       </c>
@@ -5655,7 +5662,7 @@
       </c>
       <c r="C62" s="5"/>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>0.1</v>
       </c>
@@ -5664,7 +5671,7 @@
       </c>
       <c r="C63" s="5"/>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>1.9</v>
       </c>
@@ -5673,7 +5680,7 @@
       </c>
       <c r="C64" s="5"/>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>1.1000000000000001</v>
       </c>
@@ -5682,7 +5689,7 @@
       </c>
       <c r="C65" s="5"/>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>0.6</v>
       </c>
@@ -5691,7 +5698,7 @@
       </c>
       <c r="C66" s="5"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>0.6</v>
       </c>
@@ -5700,7 +5707,7 @@
       </c>
       <c r="C67" s="5"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>1.7</v>
       </c>
@@ -5709,7 +5716,7 @@
       </c>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>2.4</v>
       </c>
@@ -5718,7 +5725,7 @@
       </c>
       <c r="C69" s="5"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>0.4</v>
       </c>
@@ -5727,7 +5734,7 @@
       </c>
       <c r="C70" s="5"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>1.2</v>
       </c>

</xml_diff>